<commit_message>
Chapter 2 tables and figures finished
</commit_message>
<xml_diff>
--- a/tables/makingTables.xlsx
+++ b/tables/makingTables.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bryce/Box Sync/n14/Writing/dissertation/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bryce/Box Sync/n14/Writing/diss/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47291E42-3276-234B-9AAD-C0F0496DA209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1402AE42-3FDE-0144-AF6A-66E3B279F243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="15020" xr2:uid="{6D9B1D0C-F512-F546-B090-1DBE6359CDA6}"/>
+    <workbookView xWindow="-28720" yWindow="-1560" windowWidth="25440" windowHeight="15020" activeTab="2" xr2:uid="{6D9B1D0C-F512-F546-B090-1DBE6359CDA6}"/>
   </bookViews>
   <sheets>
     <sheet name="sfactors" sheetId="1" r:id="rId1"/>
     <sheet name="Lifetime width" sheetId="2" r:id="rId2"/>
+    <sheet name="implantedTargets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
   <si>
     <t>Year</t>
   </si>
@@ -215,6 +216,96 @@
   </si>
   <si>
     <t>Mukhamedzhanov \textit{et al.} cite{Mukhamedzhanov2003}</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Atomic percentage</t>
+  </si>
+  <si>
+    <t>Mo (low)</t>
+  </si>
+  <si>
+    <t>Mo (mid)</t>
+  </si>
+  <si>
+    <t>Mo (high)</t>
+  </si>
+  <si>
+    <t>Ta (low)</t>
+  </si>
+  <si>
+    <t>Ta (mid)</t>
+  </si>
+  <si>
+    <t>Ta (high)</t>
+  </si>
+  <si>
+    <t>W (low)</t>
+  </si>
+  <si>
+    <t>W (mid)</t>
+  </si>
+  <si>
+    <t>W (high)</t>
+  </si>
+  <si>
+    <t>11 $\pm$ 2</t>
+  </si>
+  <si>
+    <t>14 $\pm$ 2</t>
+  </si>
+  <si>
+    <t>26 $\pm$ 5</t>
+  </si>
+  <si>
+    <t>17 $\pm$ 3</t>
+  </si>
+  <si>
+    <t>26 $\pm$ 4</t>
+  </si>
+  <si>
+    <t>36 $\pm$ 6</t>
+  </si>
+  <si>
+    <t>22 $\pm$ 4</t>
+  </si>
+  <si>
+    <t>19 $\pm$ 3</t>
+  </si>
+  <si>
+    <t>13 $\pm$ 2</t>
+  </si>
+  <si>
+    <t>Nitrogen atoms (10$^{17}$/cm$^{2}$)</t>
+  </si>
+  <si>
+    <t>5.46 $\pm$ 0.11</t>
+  </si>
+  <si>
+    <t>6.08 $\pm$ 0.12</t>
+  </si>
+  <si>
+    <t>13.10 $\pm$ 0.66</t>
+  </si>
+  <si>
+    <t>9.63 $\pm$ 0.29</t>
+  </si>
+  <si>
+    <t>14.37 $\pm$ 0.57</t>
+  </si>
+  <si>
+    <t>21.29 $\pm$ 1.28</t>
+  </si>
+  <si>
+    <t>7.33 $\pm$ 0.15</t>
+  </si>
+  <si>
+    <t>11.62 $\pm$ 0.35</t>
+  </si>
+  <si>
+    <t>13.38 $\pm$ 0.54</t>
   </si>
 </sst>
 </file>
@@ -250,11 +341,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E47A4C-B8E0-0340-BD42-AFA37995A66F}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -926,4 +1018,129 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393AF5EE-C169-9A44-A096-B0F2EF8B54EA}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added tables and a bit more explanation to target characterization section.
</commit_message>
<xml_diff>
--- a/tables/makingTables.xlsx
+++ b/tables/makingTables.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bryce/Box Sync/n14/Writing/diss/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1402AE42-3FDE-0144-AF6A-66E3B279F243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7C0BC2-74C6-5446-A0CE-738B1942F69D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28720" yWindow="-1560" windowWidth="25440" windowHeight="15020" activeTab="2" xr2:uid="{6D9B1D0C-F512-F546-B090-1DBE6359CDA6}"/>
+    <workbookView xWindow="-28720" yWindow="-1560" windowWidth="25440" windowHeight="15020" activeTab="3" xr2:uid="{6D9B1D0C-F512-F546-B090-1DBE6359CDA6}"/>
   </bookViews>
   <sheets>
     <sheet name="sfactors" sheetId="1" r:id="rId1"/>
     <sheet name="Lifetime width" sheetId="2" r:id="rId2"/>
     <sheet name="implantedTargets" sheetId="3" r:id="rId3"/>
+    <sheet name="targetThicknesses" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
   <si>
     <t>Year</t>
   </si>
@@ -306,6 +307,33 @@
   </si>
   <si>
     <t>13.38 $\pm$ 0.54</t>
+  </si>
+  <si>
+    <t>TiN</t>
+  </si>
+  <si>
+    <t>ZrN 5</t>
+  </si>
+  <si>
+    <t>ZrN 1</t>
+  </si>
+  <si>
+    <t>ZrN 12</t>
+  </si>
+  <si>
+    <t>$n$ \left(10^{17} atoms / cm^{2} \right)</t>
+  </si>
+  <si>
+    <t>7.070 $\pm$ 0.566</t>
+  </si>
+  <si>
+    <t>5.623 $\pm$ 0.450</t>
+  </si>
+  <si>
+    <t>5.826 $\pm$ 0.466</t>
+  </si>
+  <si>
+    <t>10.480 $\pm$ 0.834</t>
   </si>
 </sst>
 </file>
@@ -343,10 +371,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,13 +698,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1024,7 +1052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393AF5EE-C169-9A44-A096-B0F2EF8B54EA}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -1045,7 +1073,7 @@
       <c r="A2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C2" t="s">
@@ -1056,7 +1084,7 @@
       <c r="A3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C3" t="s">
@@ -1067,7 +1095,7 @@
       <c r="A4" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C4" t="s">
@@ -1078,7 +1106,7 @@
       <c r="A5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C5" t="s">
@@ -1089,7 +1117,7 @@
       <c r="A6" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C6" t="s">
@@ -1100,7 +1128,7 @@
       <c r="A7" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C7" t="s">
@@ -1111,7 +1139,7 @@
       <c r="A8" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C8" t="s">
@@ -1122,7 +1150,7 @@
       <c r="A9" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C9" t="s">
@@ -1133,11 +1161,66 @@
       <c r="A10" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C10" t="s">
         <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F19058F-E5CC-6B4C-8424-BA582CE98C38}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished chapter 4, including figures, tables, and citations
</commit_message>
<xml_diff>
--- a/tables/makingTables.xlsx
+++ b/tables/makingTables.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bryce/Box Sync/n14/Writing/diss/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7C0BC2-74C6-5446-A0CE-738B1942F69D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A92374B-0EA9-8247-B4EA-11C325C0AEA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28720" yWindow="-1560" windowWidth="25440" windowHeight="15020" activeTab="3" xr2:uid="{6D9B1D0C-F512-F546-B090-1DBE6359CDA6}"/>
+    <workbookView xWindow="-28720" yWindow="-1560" windowWidth="15360" windowHeight="15020" firstSheet="1" activeTab="4" xr2:uid="{6D9B1D0C-F512-F546-B090-1DBE6359CDA6}"/>
   </bookViews>
   <sheets>
     <sheet name="sfactors" sheetId="1" r:id="rId1"/>
     <sheet name="Lifetime width" sheetId="2" r:id="rId2"/>
     <sheet name="implantedTargets" sheetId="3" r:id="rId3"/>
     <sheet name="targetThicknesses" sheetId="4" r:id="rId4"/>
+    <sheet name="518" sheetId="5" r:id="rId5"/>
+    <sheet name="617" sheetId="6" r:id="rId6"/>
+    <sheet name="679" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="131">
   <si>
     <t>Year</t>
   </si>
@@ -334,19 +337,118 @@
   </si>
   <si>
     <t>10.480 $\pm$ 0.834</t>
+  </si>
+  <si>
+    <t>Mo Implanted Target</t>
+  </si>
+  <si>
+    <t>Ta Implanted Target</t>
+  </si>
+  <si>
+    <t>W Implanted Target</t>
+  </si>
+  <si>
+    <t>$F(\tau)_{5.18}$</t>
+  </si>
+  <si>
+    <t>$9.04 \pm 0.013$</t>
+  </si>
+  <si>
+    <t>$0.911 \pm 0.016$</t>
+  </si>
+  <si>
+    <t>$9.12 \pm 0.015$</t>
+  </si>
+  <si>
+    <t>$﻿7.1^{+4.8}_{-2.3}$</t>
+  </si>
+  <si>
+    <t>Weighted Average</t>
+  </si>
+  <si>
+    <t>$8.0 \pm 6.7$</t>
+  </si>
+  <si>
+    <t>$7.1 \pm 5.5$</t>
+  </si>
+  <si>
+    <t>$7.5 \pm 3.0$</t>
+  </si>
+  <si>
+    <t>$F(\tau)_{6.17}$</t>
+  </si>
+  <si>
+    <t>$F(\tau)_{6.79}$</t>
+  </si>
+  <si>
+    <t>$0.992 \pm 0.014$</t>
+  </si>
+  <si>
+    <t>$0.976 \pm 0.017$</t>
+  </si>
+  <si>
+    <t>$0.988 \pm 0.016$</t>
+  </si>
+  <si>
+    <t>$0.4^{+0.7}_{-0.4}$</t>
+  </si>
+  <si>
+    <t>$1.4 \pm 1.0$</t>
+  </si>
+  <si>
+    <t>$0.6^{+0.9}_{-0.6}$</t>
+  </si>
+  <si>
+    <t>$0.7 \pm 0.5$</t>
+  </si>
+  <si>
+    <t>$0.995 \pm 0.019$</t>
+  </si>
+  <si>
+    <t>$ 0.983 \pm 0.019$</t>
+  </si>
+  <si>
+    <t>$0.978 \pm 0.015$</t>
+  </si>
+  <si>
+    <t>$0.2^{+0.7}_{-0.2}$</t>
+  </si>
+  <si>
+    <t>$0.7^{+0.9}_{-0.7}$</t>
+  </si>
+  <si>
+    <t>$0.9 \pm 0.6$</t>
+  </si>
+  <si>
+    <t>$\tau_{6.79}$ (fs)</t>
+  </si>
+  <si>
+    <t>$0.6 \pm 0.4$</t>
+  </si>
+  <si>
+    <t>$\tau_{6.17}$ (fs)</t>
+  </si>
+  <si>
+    <t>$\tau_{5.18}$ (fs)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF61CE3C"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -369,12 +471,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,7 +1280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F19058F-E5CC-6B4C-8424-BA582CE98C38}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
@@ -1226,4 +1329,184 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35073415-4BC8-F74D-ACDB-7AF364D1DF27}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8403B6-7C22-924B-BABA-AB3CE1111880}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A8B8EF-2EC7-DA48-8C2D-F8181AB09D0C}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>